<commit_message>
All trees now start as colapsed
</commit_message>
<xml_diff>
--- a/src/main/java/org/openepics/names/services/NamingDatabaseImport.xlsx
+++ b/src/main/java/org/openepics/names/services/NamingDatabaseImport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="780" windowWidth="34875" windowHeight="16320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="975" yWindow="780" windowWidth="34875" windowHeight="16320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogicalAreaStructure" sheetId="3" r:id="rId1"/>
@@ -5892,7 +5892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
@@ -8493,10 +8493,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E941"/>
+  <dimension ref="A1:E940"/>
   <sheetViews>
-    <sheetView topLeftCell="A902" workbookViewId="0">
-      <selection activeCell="D943" sqref="D943"/>
+    <sheetView tabSelected="1" topLeftCell="A919" workbookViewId="0">
+      <selection activeCell="E942" sqref="E942"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -20383,65 +20383,54 @@
     </row>
     <row r="937" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A937" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B937" s="2">
-        <v>13307</v>
+        <v>13308</v>
       </c>
       <c r="C937" s="2">
-        <v>23034</v>
+        <v>23035</v>
+      </c>
+      <c r="D937" s="1" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="938" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A938" s="2">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B938" s="2">
         <v>13308</v>
       </c>
       <c r="C938" s="2">
-        <v>23035</v>
-      </c>
-      <c r="D938" s="1" t="s">
-        <v>636</v>
+        <v>23039</v>
       </c>
     </row>
     <row r="939" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A939" s="2">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B939" s="2">
         <v>13308</v>
       </c>
       <c r="C939" s="2">
-        <v>23039</v>
+        <v>23035</v>
+      </c>
+      <c r="D939" s="1" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="940" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A940" s="2">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B940" s="2">
         <v>13308</v>
       </c>
       <c r="C940" s="2">
-        <v>23035</v>
-      </c>
-      <c r="D940" s="1" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="941" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A941" s="2">
-        <v>940</v>
-      </c>
-      <c r="B941" s="2">
-        <v>13308</v>
-      </c>
-      <c r="C941" s="2">
         <v>23033</v>
       </c>
-      <c r="D941" t="s">
+      <c r="D940" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>